<commit_message>
Made a demand figure and added presentation file
</commit_message>
<xml_diff>
--- a/MESSAGEix_South_Africa/Data/SSP5/SSP5_data.xlsx
+++ b/MESSAGEix_South_Africa/Data/SSP5/SSP5_data.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jansn\GitHub\SSP5_Clone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jansn\GitHub\SSP5_Clone\MESSAGEix_South_Africa\Data\SSP5\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -585,19 +586,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -607,6 +602,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -624,6 +625,2935 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nb-NO"/>
+              <a:t>Final</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="nb-NO" baseline="0"/>
+              <a:t> e</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="nb-NO"/>
+              <a:t>nergy demand - SSP5 Africa</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nb-NO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Baseline</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$F$6:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2050</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2060</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2070</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2080</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2090</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$6:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>44.52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>69.23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>86.82</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>115.99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150.18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>181.26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>213.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>243.12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>260.57</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>277.90999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-6023-4CA5-98A4-83953E1AF4E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>RCP 6.0</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$6:$O$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>44.52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.680000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82.13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>103.52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>133.26999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>158.78</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>184.97</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>208.49</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>222.86</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>240.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000001D-6023-4CA5-98A4-83953E1AF4E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>RCP 4.5</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$6:$O$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>44.52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.680000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82.13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>103.52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>133.26999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>158.78</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>184.97</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>208.49</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>222.86</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>240.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000001E-6023-4CA5-98A4-83953E1AF4E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>RCP 3.4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$W$6:$W$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>44.52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.680000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78.31</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>92.26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>115.16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>130.63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>148.22999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>170.66</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>192.21</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>212.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000001F-6023-4CA5-98A4-83953E1AF4E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>RCP 2.6</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AA$6:$AA$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>44.52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.680000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78.48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>87.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>105.14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>119.44</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>140.09</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>162.49</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>188.55</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>212.42000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000020-6023-4CA5-98A4-83953E1AF4E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>RCP 1.9</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AE$6:$AE$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>44.52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.680000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70.61</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>69.180000000000007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>86.11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>103.58000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>131.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>159.69</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>185.72</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>208.15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000021-6023-4CA5-98A4-83953E1AF4E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="433280760"/>
+        <c:axId val="433286008"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="433280760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nb-NO"/>
+                  <a:t>Year</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nb-NO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="433286008"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="433286008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nb-NO"/>
+                  <a:t>EJ</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nb-NO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="433280760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nb-NO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nb-NO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nb-NO"/>
+              <a:t>Final</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="nb-NO" baseline="0"/>
+              <a:t> e</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="nb-NO"/>
+              <a:t>nergy demand - SSP5 Africa</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nb-NO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Baseline</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$F$6:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2050</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2060</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2070</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2080</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2090</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$6:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>44.52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>69.23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>86.82</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>115.99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150.18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>181.26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>213.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>243.12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>260.57</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>277.90999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7DD4-42B4-93D8-42FF586445EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>RCP 6.0</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$6:$O$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>44.52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.680000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82.13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>103.52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>133.26999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>158.78</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>184.97</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>208.49</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>222.86</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>240.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7DD4-42B4-93D8-42FF586445EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>RCP 4.5</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$6:$O$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>44.52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.680000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82.13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>103.52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>133.26999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>158.78</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>184.97</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>208.49</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>222.86</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>240.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7DD4-42B4-93D8-42FF586445EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>RCP 3.4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$W$6:$W$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>44.52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.680000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78.31</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>92.26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>115.16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>130.63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>148.22999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>170.66</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>192.21</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>212.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-7DD4-42B4-93D8-42FF586445EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>RCP 2.6</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AA$6:$AA$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>44.52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.680000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78.48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>87.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>105.14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>119.44</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>140.09</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>162.49</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>188.55</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>212.42000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-7DD4-42B4-93D8-42FF586445EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>RCP 1.9</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AE$6:$AE$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>44.52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.680000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70.61</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>69.180000000000007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>86.11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>103.58000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>131.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>159.69</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>185.72</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>208.15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-7DD4-42B4-93D8-42FF586445EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="433280760"/>
+        <c:axId val="433286008"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="433280760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nb-NO"/>
+                  <a:t>Year</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nb-NO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="433286008"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="433286008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nb-NO"/>
+                  <a:t>EJ</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nb-NO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="433280760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nb-NO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nb-NO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -891,11 +3821,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BE15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="AF6" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="5" topLeftCell="AS6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AN7" sqref="AN7"/>
+      <selection pane="bottomRight" activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -935,140 +3865,140 @@
       <c r="G2" s="41"/>
       <c r="H2" s="41"/>
       <c r="I2" s="42"/>
-      <c r="J2" s="48" t="s">
+      <c r="J2" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="49"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="49"/>
-      <c r="W2" s="49"/>
-      <c r="X2" s="49"/>
-      <c r="Y2" s="49"/>
-      <c r="Z2" s="49"/>
-      <c r="AA2" s="49"/>
-      <c r="AB2" s="49"/>
-      <c r="AC2" s="49"/>
-      <c r="AD2" s="49"/>
-      <c r="AE2" s="49"/>
-      <c r="AF2" s="49"/>
-      <c r="AG2" s="50"/>
-      <c r="AH2" s="48" t="s">
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
+      <c r="V2" s="47"/>
+      <c r="W2" s="47"/>
+      <c r="X2" s="47"/>
+      <c r="Y2" s="47"/>
+      <c r="Z2" s="47"/>
+      <c r="AA2" s="47"/>
+      <c r="AB2" s="47"/>
+      <c r="AC2" s="47"/>
+      <c r="AD2" s="47"/>
+      <c r="AE2" s="47"/>
+      <c r="AF2" s="47"/>
+      <c r="AG2" s="48"/>
+      <c r="AH2" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="AI2" s="49"/>
-      <c r="AJ2" s="49"/>
-      <c r="AK2" s="49"/>
-      <c r="AL2" s="49"/>
-      <c r="AM2" s="49"/>
-      <c r="AN2" s="49"/>
-      <c r="AO2" s="49"/>
-      <c r="AP2" s="49"/>
-      <c r="AQ2" s="49"/>
-      <c r="AR2" s="49"/>
-      <c r="AS2" s="49"/>
-      <c r="AT2" s="49"/>
-      <c r="AU2" s="49"/>
-      <c r="AV2" s="49"/>
-      <c r="AW2" s="49"/>
-      <c r="AX2" s="49"/>
-      <c r="AY2" s="49"/>
-      <c r="AZ2" s="49"/>
-      <c r="BA2" s="49"/>
-      <c r="BB2" s="49"/>
-      <c r="BC2" s="49"/>
-      <c r="BD2" s="49"/>
-      <c r="BE2" s="50"/>
+      <c r="AI2" s="47"/>
+      <c r="AJ2" s="47"/>
+      <c r="AK2" s="47"/>
+      <c r="AL2" s="47"/>
+      <c r="AM2" s="47"/>
+      <c r="AN2" s="47"/>
+      <c r="AO2" s="47"/>
+      <c r="AP2" s="47"/>
+      <c r="AQ2" s="47"/>
+      <c r="AR2" s="47"/>
+      <c r="AS2" s="47"/>
+      <c r="AT2" s="47"/>
+      <c r="AU2" s="47"/>
+      <c r="AV2" s="47"/>
+      <c r="AW2" s="47"/>
+      <c r="AX2" s="47"/>
+      <c r="AY2" s="47"/>
+      <c r="AZ2" s="47"/>
+      <c r="BA2" s="47"/>
+      <c r="BB2" s="47"/>
+      <c r="BC2" s="47"/>
+      <c r="BD2" s="47"/>
+      <c r="BE2" s="48"/>
     </row>
     <row r="3" spans="2:57" s="37" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F3" s="38"/>
       <c r="G3" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="44"/>
-      <c r="J3" s="45" t="s">
+      <c r="I3" s="50"/>
+      <c r="J3" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="47" t="s">
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="47" t="s">
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="45"/>
+      <c r="R3" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="46"/>
-      <c r="V3" s="47" t="s">
+      <c r="S3" s="44"/>
+      <c r="T3" s="44"/>
+      <c r="U3" s="45"/>
+      <c r="V3" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="W3" s="45"/>
-      <c r="X3" s="45"/>
-      <c r="Y3" s="46"/>
-      <c r="Z3" s="47" t="s">
+      <c r="W3" s="44"/>
+      <c r="X3" s="44"/>
+      <c r="Y3" s="45"/>
+      <c r="Z3" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="AA3" s="45"/>
-      <c r="AB3" s="45"/>
-      <c r="AC3" s="46"/>
-      <c r="AD3" s="47" t="s">
+      <c r="AA3" s="44"/>
+      <c r="AB3" s="44"/>
+      <c r="AC3" s="45"/>
+      <c r="AD3" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="AE3" s="45"/>
-      <c r="AF3" s="45"/>
-      <c r="AG3" s="46"/>
-      <c r="AH3" s="47" t="s">
+      <c r="AE3" s="44"/>
+      <c r="AF3" s="44"/>
+      <c r="AG3" s="45"/>
+      <c r="AH3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="AI3" s="45"/>
-      <c r="AJ3" s="45"/>
-      <c r="AK3" s="46"/>
-      <c r="AL3" s="47" t="s">
+      <c r="AI3" s="44"/>
+      <c r="AJ3" s="44"/>
+      <c r="AK3" s="45"/>
+      <c r="AL3" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="AM3" s="45"/>
-      <c r="AN3" s="45"/>
-      <c r="AO3" s="46"/>
-      <c r="AP3" s="47" t="s">
+      <c r="AM3" s="44"/>
+      <c r="AN3" s="44"/>
+      <c r="AO3" s="45"/>
+      <c r="AP3" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="AQ3" s="45"/>
-      <c r="AR3" s="45"/>
-      <c r="AS3" s="46"/>
-      <c r="AT3" s="47" t="s">
+      <c r="AQ3" s="44"/>
+      <c r="AR3" s="44"/>
+      <c r="AS3" s="45"/>
+      <c r="AT3" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="AU3" s="45"/>
-      <c r="AV3" s="45"/>
-      <c r="AW3" s="46"/>
-      <c r="AX3" s="47" t="s">
+      <c r="AU3" s="44"/>
+      <c r="AV3" s="44"/>
+      <c r="AW3" s="45"/>
+      <c r="AX3" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="AY3" s="45"/>
-      <c r="AZ3" s="45"/>
-      <c r="BA3" s="46"/>
-      <c r="BB3" s="47" t="s">
+      <c r="AY3" s="44"/>
+      <c r="AZ3" s="44"/>
+      <c r="BA3" s="45"/>
+      <c r="BB3" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="BC3" s="45"/>
-      <c r="BD3" s="45"/>
-      <c r="BE3" s="46"/>
+      <c r="BC3" s="44"/>
+      <c r="BD3" s="44"/>
+      <c r="BE3" s="45"/>
     </row>
     <row r="4" spans="2:57" s="18" customFormat="1" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="34" t="s">
@@ -3303,6 +6233,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="V3:Y3"/>
+    <mergeCell ref="Z3:AC3"/>
+    <mergeCell ref="N3:Q3"/>
     <mergeCell ref="AD3:AG3"/>
     <mergeCell ref="J2:AG2"/>
     <mergeCell ref="AH2:BE2"/>
@@ -3312,14 +6248,23 @@
     <mergeCell ref="AX3:BA3"/>
     <mergeCell ref="BB3:BE3"/>
     <mergeCell ref="AL3:AO3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="V3:Y3"/>
-    <mergeCell ref="Z3:AC3"/>
-    <mergeCell ref="N3:Q3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>